<commit_message>
Added the review comments need to Update the script
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-Settings.xlsx
+++ b/tests/artifact/script/UI-Settings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="620" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6830" tabRatio="620" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="1004">
   <si>
     <t>target</t>
   </si>
@@ -2527,6 +2527,9 @@
     <t xml:space="preserve">Click Transaction tab - Save Button </t>
   </si>
   <si>
+    <t>After saving Transaction still the settings page is visible right? Then why we need to click again settings</t>
+  </si>
+  <si>
     <t>Verify Manager Users Page</t>
   </si>
   <si>
@@ -2536,6 +2539,9 @@
     <t>${org.ManageUser}</t>
   </si>
   <si>
+    <t>We can verify any one or two Field level validation</t>
+  </si>
+  <si>
     <t>Assert Invite button</t>
   </si>
   <si>
@@ -2560,6 +2566,9 @@
     <t>${Users.Table}</t>
   </si>
   <si>
+    <t>Use go back to the previous page and click on Organisation menu</t>
+  </si>
+  <si>
     <t>Assert Invitations Table</t>
   </si>
   <si>
@@ -2569,6 +2578,9 @@
     <t>Verify Organization tab</t>
   </si>
   <si>
+    <t>After Navigating Organisation page, how do we know we are in Organisation any validations?</t>
+  </si>
+  <si>
     <t>Click Organization tab</t>
   </si>
   <si>
@@ -2674,6 +2686,9 @@
     <t>${Validate.button}</t>
   </si>
   <si>
+    <t>After clicking Autofill How we can verify the table? wheather it is present or not.</t>
+  </si>
+  <si>
     <t>Click on Autofill button</t>
   </si>
   <si>
@@ -2689,6 +2704,9 @@
     <t>HDFC98765432024</t>
   </si>
   <si>
+    <t>Where is the validation of Validate &amp; AutoFill Button After this step</t>
+  </si>
+  <si>
     <t>Enter GSTIN number</t>
   </si>
   <si>
@@ -2725,6 +2743,9 @@
     <t>${Organization.CessButton}</t>
   </si>
   <si>
+    <t>After entering the CESS Where is the cancel validation</t>
+  </si>
+  <si>
     <t>Enter the CESS percentage</t>
   </si>
   <si>
@@ -2737,12 +2758,18 @@
     <t>${Organization.CessAdd}</t>
   </si>
   <si>
+    <t>After adding CESS There is delete button are you covered in this?</t>
+  </si>
+  <si>
     <t>Click on Save Changes button</t>
   </si>
   <si>
     <t>${Organization.SaveChanges}</t>
   </si>
   <si>
+    <t>Where is Delete Organisation button validation and Confirmation POP up Message</t>
+  </si>
+  <si>
     <t>Verify the Confirmation Message</t>
   </si>
   <si>
@@ -2764,6 +2791,9 @@
     <t>${Org.Name} Profile Details Updated</t>
   </si>
   <si>
+    <t>After that you can use go back button right?</t>
+  </si>
+  <si>
     <t>Verify the Success Message</t>
   </si>
   <si>
@@ -2866,6 +2896,9 @@
     <t>${user.home}\Downloads\${xlsxFileName}.xlsx</t>
   </si>
   <si>
+    <t>U can use Go bcak to the previous button</t>
+  </si>
+  <si>
     <t>${user.home}\Downloads\${jsonFileName}.json</t>
   </si>
   <si>
@@ -2972,6 +3005,9 @@
   </si>
   <si>
     <t>${Org.ImportData.Link1}</t>
+  </si>
+  <si>
+    <t>Where is validation of Links Tally &amp; GNUKhata and JSON</t>
   </si>
   <si>
     <t>${Org.ImportData.Link2}</t>
@@ -3048,12 +3084,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="39">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3137,15 +3173,20 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
-      <color theme="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Tahoma"/>
@@ -3156,6 +3197,14 @@
       <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3668,147 +3717,147 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -4010,32 +4059,50 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -4044,6 +4111,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4060,7 +4131,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -7112,7 +7183,7 @@
   <sheetPr/>
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
@@ -7263,7 +7334,7 @@
       <c r="E5" s="22" t="s">
         <v>747</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="80" t="s">
         <v>748</v>
       </c>
       <c r="G5" s="22"/>
@@ -7348,7 +7419,7 @@
       <c r="O12" s="17"/>
     </row>
     <row r="13" ht="19" customHeight="1" spans="6:6">
-      <c r="F13" s="74"/>
+      <c r="F13" s="81"/>
     </row>
     <row r="14" ht="21" customHeight="1"/>
     <row r="15" ht="22" customHeight="1"/>
@@ -7406,9 +7477,9 @@
     <row r="19" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="27"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="77"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="84"/>
       <c r="F19" s="25"/>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -7438,10 +7509,10 @@
       <c r="O20" s="17"/>
     </row>
     <row r="21" s="41" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A21" s="78"/>
-      <c r="B21" s="79"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="76"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="83"/>
       <c r="E21" s="46"/>
       <c r="F21" s="46"/>
       <c r="G21" s="46"/>
@@ -7629,12 +7700,12 @@
       <c r="O32" s="17"/>
     </row>
     <row r="33" s="41" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A33" s="78"/>
-      <c r="B33" s="79"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="77"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="84"/>
       <c r="E33" s="46"/>
-      <c r="F33" s="81"/>
+      <c r="F33" s="88"/>
       <c r="G33" s="46"/>
       <c r="H33" s="46"/>
       <c r="I33" s="46"/>
@@ -7646,9 +7717,9 @@
       <c r="O33" s="49"/>
     </row>
     <row r="34" s="41" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A34" s="78"/>
-      <c r="B34" s="79"/>
-      <c r="C34" s="80"/>
+      <c r="A34" s="85"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="87"/>
       <c r="D34" s="46"/>
       <c r="E34" s="46"/>
       <c r="F34" s="46"/>
@@ -10496,10 +10567,10 @@
   <sheetPr/>
   <dimension ref="A1:O267"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
@@ -11449,8 +11520,10 @@
       <c r="N34" s="39"/>
       <c r="O34" s="29"/>
     </row>
-    <row r="35" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A35" s="27"/>
+    <row r="35" s="6" customFormat="1" ht="65" customHeight="1" spans="1:15">
+      <c r="A35" s="62" t="s">
+        <v>820</v>
+      </c>
       <c r="B35" s="20" t="s">
         <v>794</v>
       </c>
@@ -11478,7 +11551,7 @@
     </row>
     <row r="36" s="6" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A36" s="27" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>761</v>
@@ -11507,7 +11580,7 @@
     </row>
     <row r="37" s="5" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B37" s="15" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C37" s="21" t="s">
         <v>30</v>
@@ -11516,7 +11589,7 @@
         <v>576</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="F37" s="23">
         <v>2000</v>
@@ -11531,18 +11604,21 @@
       <c r="N37" s="18"/>
       <c r="O37" s="17"/>
     </row>
-    <row r="38" s="5" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B38" s="20" t="s">
-        <v>823</v>
-      </c>
-      <c r="C38" s="21" t="s">
+    <row r="38" s="5" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="A38" s="63" t="s">
+        <v>824</v>
+      </c>
+      <c r="B38" s="64" t="s">
+        <v>825</v>
+      </c>
+      <c r="C38" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E38" s="62" t="s">
-        <v>824</v>
+      <c r="E38" s="67" t="s">
+        <v>826</v>
       </c>
       <c r="F38" s="23"/>
       <c r="G38" s="22"/>
@@ -11556,17 +11632,17 @@
       <c r="O38" s="17"/>
     </row>
     <row r="39" s="6" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B39" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="C39" s="21" t="s">
+      <c r="B39" s="64" t="s">
+        <v>827</v>
+      </c>
+      <c r="C39" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>826</v>
+      <c r="E39" s="68" t="s">
+        <v>828</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
@@ -11581,17 +11657,17 @@
     </row>
     <row r="40" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A40" s="27"/>
-      <c r="B40" s="20" t="s">
-        <v>827</v>
-      </c>
-      <c r="C40" s="21" t="s">
+      <c r="B40" s="64" t="s">
+        <v>829</v>
+      </c>
+      <c r="C40" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>828</v>
+      <c r="E40" s="68" t="s">
+        <v>830</v>
       </c>
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
@@ -11606,17 +11682,17 @@
     </row>
     <row r="41" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A41" s="27"/>
-      <c r="B41" s="20" t="s">
-        <v>829</v>
-      </c>
-      <c r="C41" s="21" t="s">
+      <c r="B41" s="64" t="s">
+        <v>831</v>
+      </c>
+      <c r="C41" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>830</v>
+      <c r="E41" s="68" t="s">
+        <v>832</v>
       </c>
       <c r="F41" s="25"/>
       <c r="G41" s="25"/>
@@ -11630,18 +11706,20 @@
       <c r="O41" s="29"/>
     </row>
     <row r="42" s="6" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A42" s="27"/>
-      <c r="B42" s="20" t="s">
-        <v>831</v>
-      </c>
-      <c r="C42" s="21" t="s">
+      <c r="A42" s="62" t="s">
+        <v>833</v>
+      </c>
+      <c r="B42" s="64" t="s">
+        <v>834</v>
+      </c>
+      <c r="C42" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>832</v>
+      <c r="E42" s="68" t="s">
+        <v>835</v>
       </c>
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
@@ -11656,7 +11734,7 @@
     </row>
     <row r="43" s="6" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A43" s="27" t="s">
-        <v>833</v>
+        <v>836</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>761</v>
@@ -11683,9 +11761,12 @@
       <c r="N43" s="39"/>
       <c r="O43" s="29"/>
     </row>
-    <row r="44" s="5" customFormat="1" ht="24" customHeight="1" spans="2:15">
+    <row r="44" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
+      <c r="A44" s="63" t="s">
+        <v>837</v>
+      </c>
       <c r="B44" s="20" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>30</v>
@@ -11694,7 +11775,7 @@
         <v>576</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="F44" s="23">
         <v>2000</v>
@@ -11712,7 +11793,7 @@
     <row r="45" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A45" s="27"/>
       <c r="B45" s="20" t="s">
-        <v>836</v>
+        <v>840</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>30</v>
@@ -11721,10 +11802,10 @@
         <v>711</v>
       </c>
       <c r="E45" t="s">
-        <v>837</v>
+        <v>841</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>838</v>
+        <v>842</v>
       </c>
       <c r="G45" s="22"/>
       <c r="H45" s="22"/>
@@ -11739,7 +11820,7 @@
     <row r="46" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A46" s="27"/>
       <c r="B46" s="20" t="s">
-        <v>839</v>
+        <v>843</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>30</v>
@@ -11748,10 +11829,10 @@
         <v>706</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>840</v>
-      </c>
-      <c r="F46" s="63" t="s">
-        <v>841</v>
+        <v>844</v>
+      </c>
+      <c r="F46" s="69" t="s">
+        <v>845</v>
       </c>
       <c r="G46" s="22"/>
       <c r="H46" s="22"/>
@@ -11775,7 +11856,7 @@
         <v>714</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>842</v>
+        <v>846</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="22"/>
@@ -11790,7 +11871,7 @@
     <row r="48" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A48" s="27"/>
       <c r="B48" s="20" t="s">
-        <v>843</v>
+        <v>847</v>
       </c>
       <c r="C48" s="21" t="s">
         <v>30</v>
@@ -11799,10 +11880,10 @@
         <v>706</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>844</v>
-      </c>
-      <c r="F48" s="63" t="s">
-        <v>845</v>
+        <v>848</v>
+      </c>
+      <c r="F48" s="69" t="s">
+        <v>849</v>
       </c>
       <c r="G48" s="22"/>
       <c r="H48" s="22"/>
@@ -11817,7 +11898,7 @@
     <row r="49" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A49" s="27"/>
       <c r="B49" s="20" t="s">
-        <v>846</v>
+        <v>850</v>
       </c>
       <c r="C49" s="21" t="s">
         <v>30</v>
@@ -11826,10 +11907,10 @@
         <v>706</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>847</v>
+        <v>851</v>
       </c>
       <c r="F49" s="26" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="22"/>
@@ -11844,7 +11925,7 @@
     <row r="50" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A50" s="27"/>
       <c r="B50" s="20" t="s">
-        <v>849</v>
+        <v>853</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>30</v>
@@ -11853,10 +11934,10 @@
         <v>706</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>850</v>
+        <v>854</v>
       </c>
       <c r="F50" s="26" t="s">
-        <v>851</v>
+        <v>855</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="22"/>
@@ -11871,7 +11952,7 @@
     <row r="51" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A51" s="27"/>
       <c r="B51" s="20" t="s">
-        <v>852</v>
+        <v>856</v>
       </c>
       <c r="C51" s="21" t="s">
         <v>30</v>
@@ -11880,10 +11961,10 @@
         <v>692</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="G51" s="22"/>
       <c r="H51" s="22"/>
@@ -11898,7 +11979,7 @@
     <row r="52" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A52" s="27"/>
       <c r="B52" s="20" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="C52" s="21" t="s">
         <v>30</v>
@@ -11907,10 +11988,10 @@
         <v>706</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="G52" s="22"/>
       <c r="H52" s="22"/>
@@ -11925,7 +12006,7 @@
     <row r="53" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A53" s="27"/>
       <c r="B53" s="20" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>30</v>
@@ -11934,7 +12015,7 @@
         <v>706</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="F53" s="23">
         <v>400070</v>
@@ -11952,7 +12033,7 @@
     <row r="54" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A54" s="27"/>
       <c r="B54" s="20" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="C54" s="21" t="s">
         <v>30</v>
@@ -11961,7 +12042,7 @@
         <v>706</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="F54" s="23">
         <v>1234567890</v>
@@ -11979,7 +12060,7 @@
     <row r="55" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A55" s="27"/>
       <c r="B55" s="20" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="C55" s="21" t="s">
         <v>30</v>
@@ -11988,7 +12069,7 @@
         <v>706</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
       <c r="F55" s="23">
         <v>1234567890</v>
@@ -12006,7 +12087,7 @@
     <row r="56" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A56" s="27"/>
       <c r="B56" s="20" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
       <c r="C56" s="43" t="s">
         <v>30</v>
@@ -12015,10 +12096,10 @@
         <v>706</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="F56" s="45" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="22"/>
@@ -12033,7 +12114,7 @@
     <row r="57" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A57" s="27"/>
       <c r="B57" s="20" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="C57" s="43" t="s">
         <v>30</v>
@@ -12042,7 +12123,7 @@
         <v>576</v>
       </c>
       <c r="E57" s="22" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="F57" s="45">
         <v>1000</v>
@@ -12058,9 +12139,11 @@
       <c r="O57" s="17"/>
     </row>
     <row r="58" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
-      <c r="A58" s="27"/>
+      <c r="A58" s="62" t="s">
+        <v>873</v>
+      </c>
       <c r="B58" s="20" t="s">
-        <v>869</v>
+        <v>874</v>
       </c>
       <c r="C58" s="43" t="s">
         <v>30</v>
@@ -12069,7 +12152,7 @@
         <v>576</v>
       </c>
       <c r="E58" s="22" t="s">
-        <v>870</v>
+        <v>875</v>
       </c>
       <c r="F58" s="45">
         <v>1000</v>
@@ -12087,7 +12170,7 @@
     <row r="59" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A59" s="27"/>
       <c r="B59" s="20" t="s">
-        <v>871</v>
+        <v>876</v>
       </c>
       <c r="C59" s="43" t="s">
         <v>30</v>
@@ -12096,10 +12179,10 @@
         <v>706</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="F59" s="26" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="G59" s="22"/>
       <c r="H59" s="22"/>
@@ -12112,9 +12195,11 @@
       <c r="O59" s="17"/>
     </row>
     <row r="60" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
-      <c r="A60" s="27"/>
+      <c r="A60" s="62" t="s">
+        <v>879</v>
+      </c>
       <c r="B60" s="20" t="s">
-        <v>874</v>
+        <v>880</v>
       </c>
       <c r="C60" s="43" t="s">
         <v>30</v>
@@ -12123,10 +12208,10 @@
         <v>706</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>875</v>
+        <v>881</v>
       </c>
       <c r="F60" s="45" t="s">
-        <v>876</v>
+        <v>882</v>
       </c>
       <c r="G60" s="22"/>
       <c r="H60" s="22"/>
@@ -12141,7 +12226,7 @@
     <row r="61" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A61" s="27"/>
       <c r="B61" s="20" t="s">
-        <v>877</v>
+        <v>883</v>
       </c>
       <c r="C61" s="43" t="s">
         <v>30</v>
@@ -12150,10 +12235,10 @@
         <v>563</v>
       </c>
       <c r="E61" s="45" t="s">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="F61" s="22" t="s">
-        <v>879</v>
+        <v>885</v>
       </c>
       <c r="G61" s="22"/>
       <c r="H61" s="22"/>
@@ -12168,7 +12253,7 @@
     <row r="62" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A62" s="27"/>
       <c r="B62" s="20" t="s">
-        <v>880</v>
+        <v>886</v>
       </c>
       <c r="C62" s="43" t="s">
         <v>30</v>
@@ -12177,10 +12262,10 @@
         <v>706</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>881</v>
+        <v>887</v>
       </c>
       <c r="F62" s="45" t="s">
-        <v>876</v>
+        <v>882</v>
       </c>
       <c r="G62" s="22"/>
       <c r="H62" s="22"/>
@@ -12195,7 +12280,7 @@
     <row r="63" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A63" s="27"/>
       <c r="B63" s="20" t="s">
-        <v>882</v>
+        <v>888</v>
       </c>
       <c r="C63" s="43" t="s">
         <v>30</v>
@@ -12204,7 +12289,7 @@
         <v>714</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>883</v>
+        <v>889</v>
       </c>
       <c r="F63" s="45"/>
       <c r="G63" s="22"/>
@@ -12220,7 +12305,7 @@
     <row r="64" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A64" s="27"/>
       <c r="B64" s="20" t="s">
-        <v>884</v>
+        <v>890</v>
       </c>
       <c r="C64" s="43" t="s">
         <v>30</v>
@@ -12229,7 +12314,7 @@
         <v>576</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>885</v>
+        <v>891</v>
       </c>
       <c r="F64" s="45">
         <v>1000</v>
@@ -12247,7 +12332,7 @@
     <row r="65" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A65" s="27"/>
       <c r="B65" s="20" t="s">
-        <v>882</v>
+        <v>888</v>
       </c>
       <c r="C65" s="43" t="s">
         <v>30</v>
@@ -12256,7 +12341,7 @@
         <v>714</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>883</v>
+        <v>889</v>
       </c>
       <c r="F65" s="45"/>
       <c r="G65" s="22"/>
@@ -12269,10 +12354,12 @@
       <c r="N65" s="18"/>
       <c r="O65" s="17"/>
     </row>
-    <row r="66" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
-      <c r="A66" s="27"/>
+    <row r="66" s="5" customFormat="1" ht="37" customHeight="1" spans="1:15">
+      <c r="A66" s="62" t="s">
+        <v>892</v>
+      </c>
       <c r="B66" s="20" t="s">
-        <v>886</v>
+        <v>893</v>
       </c>
       <c r="C66" s="43" t="s">
         <v>30</v>
@@ -12281,7 +12368,7 @@
         <v>706</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>887</v>
+        <v>894</v>
       </c>
       <c r="F66" s="45">
         <v>10</v>
@@ -12298,8 +12385,8 @@
     </row>
     <row r="67" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A67" s="27"/>
-      <c r="B67" s="20" t="s">
-        <v>888</v>
+      <c r="B67" s="64" t="s">
+        <v>895</v>
       </c>
       <c r="C67" s="43" t="s">
         <v>30</v>
@@ -12308,7 +12395,7 @@
         <v>576</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>889</v>
+        <v>896</v>
       </c>
       <c r="F67" s="45">
         <v>1000</v>
@@ -12323,10 +12410,12 @@
       <c r="N67" s="18"/>
       <c r="O67" s="17"/>
     </row>
-    <row r="68" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
-      <c r="A68" s="27"/>
+    <row r="68" s="5" customFormat="1" ht="31" customHeight="1" spans="1:15">
+      <c r="A68" s="62" t="s">
+        <v>897</v>
+      </c>
       <c r="B68" s="20" t="s">
-        <v>890</v>
+        <v>898</v>
       </c>
       <c r="C68" s="43" t="s">
         <v>30</v>
@@ -12335,7 +12424,7 @@
         <v>576</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>891</v>
+        <v>899</v>
       </c>
       <c r="F68" s="45">
         <v>1000</v>
@@ -12350,10 +12439,12 @@
       <c r="N68" s="18"/>
       <c r="O68" s="17"/>
     </row>
-    <row r="69" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
-      <c r="A69" s="27"/>
+    <row r="69" s="5" customFormat="1" ht="42" customHeight="1" spans="1:15">
+      <c r="A69" s="62" t="s">
+        <v>900</v>
+      </c>
       <c r="B69" s="20" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="C69" s="43" t="s">
         <v>30</v>
@@ -12362,7 +12453,7 @@
         <v>253</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>893</v>
+        <v>902</v>
       </c>
       <c r="F69" s="45"/>
       <c r="G69" s="22"/>
@@ -12378,7 +12469,7 @@
     <row r="70" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A70" s="27"/>
       <c r="B70" s="20" t="s">
-        <v>894</v>
+        <v>903</v>
       </c>
       <c r="C70" s="43" t="s">
         <v>30</v>
@@ -12387,7 +12478,7 @@
         <v>576</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>895</v>
+        <v>904</v>
       </c>
       <c r="F70" s="45">
         <v>3000</v>
@@ -12405,7 +12496,7 @@
     <row r="71" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
       <c r="A71" s="27"/>
       <c r="B71" s="20" t="s">
-        <v>896</v>
+        <v>905</v>
       </c>
       <c r="C71" s="43" t="s">
         <v>5</v>
@@ -12414,10 +12505,10 @@
         <v>471</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>897</v>
+        <v>906</v>
       </c>
       <c r="F71" s="45" t="s">
-        <v>898</v>
+        <v>907</v>
       </c>
       <c r="G71" s="22"/>
       <c r="H71" s="22"/>
@@ -12430,9 +12521,11 @@
       <c r="O71" s="17"/>
     </row>
     <row r="72" s="5" customFormat="1" ht="24" customHeight="1" spans="1:15">
-      <c r="A72" s="27"/>
+      <c r="A72" s="62" t="s">
+        <v>908</v>
+      </c>
       <c r="B72" s="20" t="s">
-        <v>899</v>
+        <v>909</v>
       </c>
       <c r="C72" s="43" t="s">
         <v>30</v>
@@ -12441,10 +12534,10 @@
         <v>530</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>901</v>
+        <v>911</v>
       </c>
       <c r="G72" s="22"/>
       <c r="H72" s="22"/>
@@ -12458,7 +12551,7 @@
     </row>
     <row r="73" s="6" customFormat="1" ht="29" customHeight="1" spans="1:15">
       <c r="A73" s="27" t="s">
-        <v>902</v>
+        <v>912</v>
       </c>
       <c r="B73" s="15" t="s">
         <v>761</v>
@@ -12487,7 +12580,7 @@
     </row>
     <row r="74" s="5" customFormat="1" ht="23" customHeight="1" spans="2:15">
       <c r="B74" s="15" t="s">
-        <v>903</v>
+        <v>913</v>
       </c>
       <c r="C74" s="21" t="s">
         <v>30</v>
@@ -12496,7 +12589,7 @@
         <v>576</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>904</v>
+        <v>914</v>
       </c>
       <c r="F74" s="23">
         <v>2000</v>
@@ -12512,17 +12605,17 @@
       <c r="O74" s="17"/>
     </row>
     <row r="75" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B75" s="20" t="s">
-        <v>905</v>
-      </c>
-      <c r="C75" s="21" t="s">
+      <c r="B75" s="64" t="s">
+        <v>915</v>
+      </c>
+      <c r="C75" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D75" s="22" t="s">
+      <c r="D75" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E75" t="s">
-        <v>906</v>
+      <c r="E75" s="68" t="s">
+        <v>916</v>
       </c>
       <c r="F75" s="25"/>
       <c r="G75" s="25"/>
@@ -12536,17 +12629,17 @@
       <c r="O75" s="29"/>
     </row>
     <row r="76" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B76" s="20" t="s">
-        <v>907</v>
-      </c>
-      <c r="C76" s="21" t="s">
+      <c r="B76" s="64" t="s">
+        <v>917</v>
+      </c>
+      <c r="C76" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D76" s="22" t="s">
+      <c r="D76" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E76" t="s">
-        <v>908</v>
+      <c r="E76" s="68" t="s">
+        <v>918</v>
       </c>
       <c r="F76" s="25"/>
       <c r="G76" s="25"/>
@@ -12560,17 +12653,17 @@
       <c r="O76" s="29"/>
     </row>
     <row r="77" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B77" s="20" t="s">
-        <v>909</v>
-      </c>
-      <c r="C77" s="21" t="s">
+      <c r="B77" s="64" t="s">
+        <v>919</v>
+      </c>
+      <c r="C77" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D77" s="22" t="s">
+      <c r="D77" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E77" t="s">
-        <v>910</v>
+      <c r="E77" s="68" t="s">
+        <v>920</v>
       </c>
       <c r="F77" s="25"/>
       <c r="G77" s="25"/>
@@ -12584,17 +12677,17 @@
       <c r="O77" s="29"/>
     </row>
     <row r="78" customFormat="1" ht="23" customHeight="1" spans="2:15">
-      <c r="B78" s="20" t="s">
-        <v>911</v>
-      </c>
-      <c r="C78" s="21" t="s">
+      <c r="B78" s="64" t="s">
+        <v>921</v>
+      </c>
+      <c r="C78" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D78" s="22" t="s">
+      <c r="D78" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E78" t="s">
-        <v>912</v>
+      <c r="E78" s="68" t="s">
+        <v>922</v>
       </c>
       <c r="F78" s="25"/>
       <c r="G78" s="25"/>
@@ -12609,7 +12702,7 @@
     </row>
     <row r="79" customFormat="1" ht="28" spans="2:15">
       <c r="B79" s="20" t="s">
-        <v>913</v>
+        <v>923</v>
       </c>
       <c r="C79" s="21" t="s">
         <v>30</v>
@@ -12618,7 +12711,7 @@
         <v>363</v>
       </c>
       <c r="E79" t="s">
-        <v>914</v>
+        <v>924</v>
       </c>
       <c r="F79" s="25"/>
       <c r="G79" s="25"/>
@@ -12632,20 +12725,20 @@
       <c r="O79" s="29"/>
     </row>
     <row r="80" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A80" s="64"/>
+      <c r="A80" s="62"/>
       <c r="B80" s="20" t="s">
-        <v>915</v>
+        <v>925</v>
       </c>
       <c r="C80" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D80" s="62" t="s">
+      <c r="D80" s="70" t="s">
         <v>540</v>
       </c>
       <c r="E80" s="20" t="s">
-        <v>916</v>
-      </c>
-      <c r="F80" s="65"/>
+        <v>926</v>
+      </c>
+      <c r="F80" s="71"/>
       <c r="G80" s="25"/>
       <c r="H80" s="25"/>
       <c r="I80" s="25"/>
@@ -12659,7 +12752,7 @@
     <row r="81" s="52" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A81" s="14"/>
       <c r="B81" s="15" t="s">
-        <v>917</v>
+        <v>927</v>
       </c>
       <c r="C81" s="21" t="s">
         <v>8</v>
@@ -12668,12 +12761,12 @@
         <v>633</v>
       </c>
       <c r="E81" s="52" t="s">
-        <v>918</v>
-      </c>
-      <c r="F81" s="66" t="s">
-        <v>919</v>
-      </c>
-      <c r="G81" s="62"/>
+        <v>928</v>
+      </c>
+      <c r="F81" s="72" t="s">
+        <v>929</v>
+      </c>
+      <c r="G81" s="70"/>
       <c r="H81" s="22"/>
       <c r="I81" s="22"/>
       <c r="J81" s="37"/>
@@ -12686,7 +12779,7 @@
     <row r="82" s="52" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A82" s="14"/>
       <c r="B82" s="20" t="s">
-        <v>920</v>
+        <v>930</v>
       </c>
       <c r="C82" s="21" t="s">
         <v>5</v>
@@ -12695,10 +12788,10 @@
         <v>536</v>
       </c>
       <c r="E82" s="53" t="s">
-        <v>921</v>
-      </c>
-      <c r="F82" s="66"/>
-      <c r="G82" s="62"/>
+        <v>931</v>
+      </c>
+      <c r="F82" s="72"/>
+      <c r="G82" s="70"/>
       <c r="H82" s="22"/>
       <c r="I82" s="22"/>
       <c r="J82" s="37"/>
@@ -12711,7 +12804,7 @@
     <row r="83" s="52" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A83" s="14"/>
       <c r="B83" s="20" t="s">
-        <v>922</v>
+        <v>932</v>
       </c>
       <c r="C83" s="21" t="s">
         <v>8</v>
@@ -12719,13 +12812,13 @@
       <c r="D83" s="22" t="s">
         <v>656</v>
       </c>
-      <c r="E83" s="66" t="s">
-        <v>923</v>
-      </c>
-      <c r="F83" s="67" t="s">
-        <v>924</v>
-      </c>
-      <c r="G83" s="62"/>
+      <c r="E83" s="72" t="s">
+        <v>933</v>
+      </c>
+      <c r="F83" s="73" t="s">
+        <v>934</v>
+      </c>
+      <c r="G83" s="70"/>
       <c r="H83" s="22"/>
       <c r="I83" s="22"/>
       <c r="J83" s="37"/>
@@ -12737,7 +12830,7 @@
     </row>
     <row r="84" s="6" customFormat="1" ht="28" spans="2:15">
       <c r="B84" s="20" t="s">
-        <v>925</v>
+        <v>935</v>
       </c>
       <c r="C84" s="21" t="s">
         <v>30</v>
@@ -12746,7 +12839,7 @@
         <v>363</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>926</v>
+        <v>936</v>
       </c>
       <c r="F84" s="25"/>
       <c r="G84" s="25"/>
@@ -12760,20 +12853,20 @@
       <c r="O84" s="29"/>
     </row>
     <row r="85" s="1" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A85" s="64"/>
+      <c r="A85" s="62"/>
       <c r="B85" s="20" t="s">
-        <v>915</v>
+        <v>925</v>
       </c>
       <c r="C85" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D85" s="62" t="s">
+      <c r="D85" s="70" t="s">
         <v>540</v>
       </c>
       <c r="E85" s="20" t="s">
-        <v>916</v>
-      </c>
-      <c r="F85" s="65"/>
+        <v>926</v>
+      </c>
+      <c r="F85" s="71"/>
       <c r="G85" s="25"/>
       <c r="H85" s="25"/>
       <c r="I85" s="25"/>
@@ -12787,7 +12880,7 @@
     <row r="86" s="52" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A86" s="14"/>
       <c r="B86" s="15" t="s">
-        <v>917</v>
+        <v>927</v>
       </c>
       <c r="C86" s="21" t="s">
         <v>8</v>
@@ -12796,12 +12889,12 @@
         <v>633</v>
       </c>
       <c r="E86" s="52" t="s">
-        <v>927</v>
-      </c>
-      <c r="F86" s="66" t="s">
-        <v>919</v>
-      </c>
-      <c r="G86" s="62"/>
+        <v>937</v>
+      </c>
+      <c r="F86" s="72" t="s">
+        <v>929</v>
+      </c>
+      <c r="G86" s="70"/>
       <c r="H86" s="22"/>
       <c r="I86" s="22"/>
       <c r="J86" s="37"/>
@@ -12814,7 +12907,7 @@
     <row r="87" s="52" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A87" s="14"/>
       <c r="B87" s="20" t="s">
-        <v>920</v>
+        <v>930</v>
       </c>
       <c r="C87" s="21" t="s">
         <v>5</v>
@@ -12823,10 +12916,10 @@
         <v>536</v>
       </c>
       <c r="E87" s="53" t="s">
-        <v>928</v>
-      </c>
-      <c r="F87" s="66"/>
-      <c r="G87" s="62"/>
+        <v>938</v>
+      </c>
+      <c r="F87" s="72"/>
+      <c r="G87" s="70"/>
       <c r="H87" s="22"/>
       <c r="I87" s="22"/>
       <c r="J87" s="37"/>
@@ -12837,9 +12930,9 @@
       <c r="O87" s="17"/>
     </row>
     <row r="88" s="52" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A88" s="68"/>
+      <c r="A88" s="74"/>
       <c r="B88" s="20" t="s">
-        <v>922</v>
+        <v>932</v>
       </c>
       <c r="C88" s="21" t="s">
         <v>8</v>
@@ -12847,11 +12940,11 @@
       <c r="D88" s="22" t="s">
         <v>656</v>
       </c>
-      <c r="E88" s="66" t="s">
-        <v>923</v>
-      </c>
-      <c r="F88" s="67" t="s">
-        <v>924</v>
+      <c r="E88" s="72" t="s">
+        <v>933</v>
+      </c>
+      <c r="F88" s="73" t="s">
+        <v>934</v>
       </c>
       <c r="G88" s="22"/>
       <c r="H88" s="22"/>
@@ -12864,9 +12957,9 @@
       <c r="O88" s="17"/>
     </row>
     <row r="89" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A89" s="68"/>
+      <c r="A89" s="74"/>
       <c r="B89" s="20" t="s">
-        <v>915</v>
+        <v>925</v>
       </c>
       <c r="C89" s="21" t="s">
         <v>5</v>
@@ -12874,11 +12967,11 @@
       <c r="D89" s="22" t="s">
         <v>540</v>
       </c>
-      <c r="E89" s="69">
+      <c r="E89" s="75">
         <v>2000</v>
       </c>
-      <c r="F89" s="66"/>
-      <c r="G89" s="62"/>
+      <c r="F89" s="72"/>
+      <c r="G89" s="70"/>
       <c r="H89" s="22"/>
       <c r="I89" s="22"/>
       <c r="J89" s="37"/>
@@ -12889,9 +12982,9 @@
       <c r="O89" s="17"/>
     </row>
     <row r="90" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A90" s="70"/>
+      <c r="A90" s="76"/>
       <c r="B90" s="20" t="s">
-        <v>929</v>
+        <v>939</v>
       </c>
       <c r="C90" s="21" t="s">
         <v>12</v>
@@ -12899,11 +12992,11 @@
       <c r="D90" s="22" t="s">
         <v>337</v>
       </c>
-      <c r="E90" s="66" t="s">
-        <v>930</v>
+      <c r="E90" s="72" t="s">
+        <v>940</v>
       </c>
       <c r="F90" s="20"/>
-      <c r="G90" s="62"/>
+      <c r="G90" s="70"/>
       <c r="H90" s="22"/>
       <c r="I90" s="22"/>
       <c r="J90" s="37"/>
@@ -12914,7 +13007,7 @@
       <c r="O90" s="17"/>
     </row>
     <row r="91" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A91" s="70"/>
+      <c r="A91" s="76"/>
       <c r="B91" s="20" t="s">
         <v>759</v>
       </c>
@@ -12924,11 +13017,11 @@
       <c r="D91" s="22" t="s">
         <v>540</v>
       </c>
-      <c r="E91" s="69">
+      <c r="E91" s="75">
         <v>3000</v>
       </c>
       <c r="F91" s="20"/>
-      <c r="G91" s="62"/>
+      <c r="G91" s="70"/>
       <c r="H91" s="22"/>
       <c r="I91" s="22"/>
       <c r="J91" s="37"/>
@@ -12939,9 +13032,9 @@
       <c r="O91" s="17"/>
     </row>
     <row r="92" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A92" s="68"/>
+      <c r="A92" s="74"/>
       <c r="B92" s="20" t="s">
-        <v>931</v>
+        <v>941</v>
       </c>
       <c r="C92" s="21" t="s">
         <v>12</v>
@@ -12949,13 +13042,13 @@
       <c r="D92" s="22" t="s">
         <v>349</v>
       </c>
-      <c r="E92" s="66" t="s">
-        <v>932</v>
-      </c>
-      <c r="F92" s="66" t="s">
-        <v>930</v>
-      </c>
-      <c r="G92" s="62"/>
+      <c r="E92" s="72" t="s">
+        <v>942</v>
+      </c>
+      <c r="F92" s="72" t="s">
+        <v>940</v>
+      </c>
+      <c r="G92" s="70"/>
       <c r="H92" s="22"/>
       <c r="I92" s="22"/>
       <c r="J92" s="37"/>
@@ -12966,9 +13059,11 @@
       <c r="O92" s="17"/>
     </row>
     <row r="93" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A93" s="68"/>
+      <c r="A93" s="74" t="s">
+        <v>943</v>
+      </c>
       <c r="B93" s="20" t="s">
-        <v>931</v>
+        <v>941</v>
       </c>
       <c r="C93" s="21" t="s">
         <v>12</v>
@@ -12976,13 +13071,13 @@
       <c r="D93" s="22" t="s">
         <v>349</v>
       </c>
-      <c r="E93" s="66" t="s">
-        <v>933</v>
-      </c>
-      <c r="F93" s="66" t="s">
-        <v>930</v>
-      </c>
-      <c r="G93" s="62"/>
+      <c r="E93" s="72" t="s">
+        <v>944</v>
+      </c>
+      <c r="F93" s="72" t="s">
+        <v>940</v>
+      </c>
+      <c r="G93" s="70"/>
       <c r="H93" s="22"/>
       <c r="I93" s="22"/>
       <c r="J93" s="37"/>
@@ -12994,10 +13089,10 @@
     </row>
     <row r="94" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A94" s="14" t="s">
-        <v>934</v>
+        <v>945</v>
       </c>
       <c r="B94" s="20" t="s">
-        <v>935</v>
+        <v>946</v>
       </c>
       <c r="C94" s="21" t="s">
         <v>30</v>
@@ -13005,13 +13100,13 @@
       <c r="D94" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="E94" s="66" t="s">
-        <v>936</v>
+      <c r="E94" s="72" t="s">
+        <v>947</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>883</v>
-      </c>
-      <c r="G94" s="62"/>
+        <v>889</v>
+      </c>
+      <c r="G94" s="70"/>
       <c r="H94" s="22"/>
       <c r="I94" s="22"/>
       <c r="J94" s="37"/>
@@ -13022,9 +13117,9 @@
       <c r="O94" s="17"/>
     </row>
     <row r="95" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A95" s="71"/>
+      <c r="A95" s="77"/>
       <c r="B95" s="20" t="s">
-        <v>937</v>
+        <v>948</v>
       </c>
       <c r="C95" s="21" t="s">
         <v>30</v>
@@ -13032,13 +13127,13 @@
       <c r="D95" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="E95" s="66" t="s">
-        <v>938</v>
+      <c r="E95" s="72" t="s">
+        <v>949</v>
       </c>
       <c r="F95" s="20" t="s">
-        <v>883</v>
-      </c>
-      <c r="G95" s="62"/>
+        <v>889</v>
+      </c>
+      <c r="G95" s="70"/>
       <c r="H95" s="22"/>
       <c r="I95" s="22"/>
       <c r="J95" s="37"/>
@@ -13049,9 +13144,9 @@
       <c r="O95" s="17"/>
     </row>
     <row r="96" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A96" s="71"/>
+      <c r="A96" s="77"/>
       <c r="B96" s="20" t="s">
-        <v>939</v>
+        <v>950</v>
       </c>
       <c r="C96" s="21" t="s">
         <v>5</v>
@@ -13059,13 +13154,13 @@
       <c r="D96" s="22" t="s">
         <v>471</v>
       </c>
-      <c r="E96" s="66" t="s">
-        <v>940</v>
+      <c r="E96" s="72" t="s">
+        <v>951</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>941</v>
-      </c>
-      <c r="G96" s="62"/>
+        <v>952</v>
+      </c>
+      <c r="G96" s="70"/>
       <c r="H96" s="22"/>
       <c r="I96" s="22"/>
       <c r="J96" s="37"/>
@@ -13076,9 +13171,9 @@
       <c r="O96" s="17"/>
     </row>
     <row r="97" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A97" s="71"/>
+      <c r="A97" s="77"/>
       <c r="B97" s="20" t="s">
-        <v>942</v>
+        <v>953</v>
       </c>
       <c r="C97" s="21" t="s">
         <v>30</v>
@@ -13086,13 +13181,13 @@
       <c r="D97" s="22" t="s">
         <v>706</v>
       </c>
-      <c r="E97" s="66" t="s">
-        <v>943</v>
+      <c r="E97" s="72" t="s">
+        <v>954</v>
       </c>
       <c r="F97" s="20" t="s">
-        <v>944</v>
-      </c>
-      <c r="G97" s="62"/>
+        <v>955</v>
+      </c>
+      <c r="G97" s="70"/>
       <c r="H97" s="22"/>
       <c r="I97" s="22"/>
       <c r="J97" s="37"/>
@@ -13104,7 +13199,7 @@
     </row>
     <row r="98" s="2" customFormat="1" spans="2:15">
       <c r="B98" s="15" t="s">
-        <v>945</v>
+        <v>956</v>
       </c>
       <c r="C98" s="21" t="s">
         <v>30</v>
@@ -13113,10 +13208,10 @@
         <v>706</v>
       </c>
       <c r="E98" s="22" t="s">
-        <v>946</v>
+        <v>957</v>
       </c>
       <c r="F98" s="23" t="s">
-        <v>947</v>
+        <v>958</v>
       </c>
       <c r="G98" s="22"/>
       <c r="H98" s="22"/>
@@ -13130,7 +13225,7 @@
     </row>
     <row r="99" s="2" customFormat="1" ht="15.5" spans="2:15">
       <c r="B99" s="15" t="s">
-        <v>948</v>
+        <v>959</v>
       </c>
       <c r="C99" s="21" t="s">
         <v>5</v>
@@ -13138,17 +13233,17 @@
       <c r="D99" s="22" t="s">
         <v>486</v>
       </c>
-      <c r="E99" s="72" t="s">
-        <v>949</v>
+      <c r="E99" s="78" t="s">
+        <v>960</v>
       </c>
       <c r="F99" s="23" t="s">
         <v>752</v>
       </c>
       <c r="G99" s="23" t="s">
-        <v>947</v>
+        <v>958</v>
       </c>
       <c r="H99" s="22" t="s">
-        <v>950</v>
+        <v>961</v>
       </c>
       <c r="I99" s="22"/>
       <c r="J99" s="37"/>
@@ -13161,7 +13256,7 @@
     <row r="100" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A100" s="14"/>
       <c r="B100" s="15" t="s">
-        <v>951</v>
+        <v>962</v>
       </c>
       <c r="C100" s="21" t="s">
         <v>30</v>
@@ -13169,8 +13264,8 @@
       <c r="D100" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="E100" s="72" t="s">
-        <v>952</v>
+      <c r="E100" s="78" t="s">
+        <v>963</v>
       </c>
       <c r="F100" s="23">
         <v>2000</v>
@@ -13186,9 +13281,9 @@
       <c r="O100" s="17"/>
     </row>
     <row r="101" s="53" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A101" s="71"/>
+      <c r="A101" s="77"/>
       <c r="B101" s="20" t="s">
-        <v>953</v>
+        <v>964</v>
       </c>
       <c r="C101" s="21" t="s">
         <v>30</v>
@@ -13196,13 +13291,13 @@
       <c r="D101" s="22" t="s">
         <v>576</v>
       </c>
-      <c r="E101" s="66" t="s">
-        <v>954</v>
+      <c r="E101" s="72" t="s">
+        <v>965</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>883</v>
-      </c>
-      <c r="G101" s="62"/>
+        <v>889</v>
+      </c>
+      <c r="G101" s="70"/>
       <c r="H101" s="22"/>
       <c r="I101" s="22"/>
       <c r="J101" s="37"/>
@@ -13229,7 +13324,7 @@
         <v>752</v>
       </c>
       <c r="G102" s="20" t="s">
-        <v>944</v>
+        <v>955</v>
       </c>
       <c r="H102" s="22" t="s">
         <v>754</v>
@@ -13298,7 +13393,7 @@
     <row r="105" s="6" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A105" s="14"/>
       <c r="B105" s="15" t="s">
-        <v>955</v>
+        <v>966</v>
       </c>
       <c r="C105" s="24" t="s">
         <v>30</v>
@@ -13375,7 +13470,7 @@
     <row r="108" s="5" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A108" s="14"/>
       <c r="B108" s="15" t="s">
-        <v>956</v>
+        <v>967</v>
       </c>
       <c r="C108" s="21" t="s">
         <v>30</v>
@@ -13384,7 +13479,7 @@
         <v>576</v>
       </c>
       <c r="E108" s="22" t="s">
-        <v>957</v>
+        <v>968</v>
       </c>
       <c r="F108" s="23">
         <v>3000</v>
@@ -13401,17 +13496,17 @@
     </row>
     <row r="109" s="5" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A109" s="14"/>
-      <c r="B109" s="15" t="s">
-        <v>958</v>
-      </c>
-      <c r="C109" s="21" t="s">
+      <c r="B109" s="79" t="s">
+        <v>969</v>
+      </c>
+      <c r="C109" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D109" s="22" t="s">
+      <c r="D109" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E109" s="22" t="s">
-        <v>959</v>
+      <c r="E109" s="66" t="s">
+        <v>970</v>
       </c>
       <c r="F109" s="22"/>
       <c r="G109" s="22"/>
@@ -13426,17 +13521,17 @@
     </row>
     <row r="110" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A110" s="14"/>
-      <c r="B110" s="15" t="s">
-        <v>960</v>
-      </c>
-      <c r="C110" s="21" t="s">
+      <c r="B110" s="79" t="s">
+        <v>971</v>
+      </c>
+      <c r="C110" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D110" s="22" t="s">
+      <c r="D110" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E110" s="22" t="s">
-        <v>961</v>
+      <c r="E110" s="66" t="s">
+        <v>972</v>
       </c>
       <c r="F110" s="22"/>
       <c r="G110" s="22"/>
@@ -13451,17 +13546,17 @@
     </row>
     <row r="111" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A111" s="14"/>
-      <c r="B111" s="15" t="s">
-        <v>960</v>
-      </c>
-      <c r="C111" s="21" t="s">
+      <c r="B111" s="79" t="s">
+        <v>971</v>
+      </c>
+      <c r="C111" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D111" s="22" t="s">
+      <c r="D111" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E111" s="22" t="s">
-        <v>962</v>
+      <c r="E111" s="66" t="s">
+        <v>973</v>
       </c>
       <c r="F111" s="22"/>
       <c r="G111" s="22"/>
@@ -13476,17 +13571,17 @@
     </row>
     <row r="112" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A112" s="14"/>
-      <c r="B112" s="15" t="s">
-        <v>963</v>
-      </c>
-      <c r="C112" s="21" t="s">
+      <c r="B112" s="79" t="s">
+        <v>974</v>
+      </c>
+      <c r="C112" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D112" s="22" t="s">
+      <c r="D112" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E112" s="22" t="s">
-        <v>964</v>
+      <c r="E112" s="66" t="s">
+        <v>975</v>
       </c>
       <c r="F112" s="22"/>
       <c r="G112" s="22"/>
@@ -13501,17 +13596,17 @@
     </row>
     <row r="113" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A113" s="14"/>
-      <c r="B113" s="15" t="s">
-        <v>963</v>
-      </c>
-      <c r="C113" s="21" t="s">
+      <c r="B113" s="79" t="s">
+        <v>974</v>
+      </c>
+      <c r="C113" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D113" s="22" t="s">
+      <c r="D113" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E113" s="22" t="s">
-        <v>965</v>
+      <c r="E113" s="66" t="s">
+        <v>976</v>
       </c>
       <c r="F113" s="22"/>
       <c r="G113" s="22"/>
@@ -13526,17 +13621,17 @@
     </row>
     <row r="114" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A114" s="14"/>
-      <c r="B114" s="15" t="s">
-        <v>963</v>
-      </c>
-      <c r="C114" s="21" t="s">
+      <c r="B114" s="79" t="s">
+        <v>974</v>
+      </c>
+      <c r="C114" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D114" s="22" t="s">
+      <c r="D114" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E114" s="22" t="s">
-        <v>966</v>
+      <c r="E114" s="66" t="s">
+        <v>977</v>
       </c>
       <c r="F114" s="22"/>
       <c r="G114" s="22"/>
@@ -13551,17 +13646,17 @@
     </row>
     <row r="115" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A115" s="14"/>
-      <c r="B115" s="15" t="s">
-        <v>963</v>
-      </c>
-      <c r="C115" s="21" t="s">
+      <c r="B115" s="79" t="s">
+        <v>974</v>
+      </c>
+      <c r="C115" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D115" s="22" t="s">
+      <c r="D115" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E115" s="22" t="s">
-        <v>967</v>
+      <c r="E115" s="66" t="s">
+        <v>978</v>
       </c>
       <c r="F115" s="22"/>
       <c r="G115" s="22"/>
@@ -13576,17 +13671,17 @@
     </row>
     <row r="116" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A116" s="14"/>
-      <c r="B116" s="15" t="s">
-        <v>963</v>
-      </c>
-      <c r="C116" s="21" t="s">
+      <c r="B116" s="79" t="s">
+        <v>974</v>
+      </c>
+      <c r="C116" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D116" s="22" t="s">
+      <c r="D116" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E116" s="22" t="s">
-        <v>968</v>
+      <c r="E116" s="66" t="s">
+        <v>979</v>
       </c>
       <c r="F116" s="22"/>
       <c r="G116" s="22"/>
@@ -13600,18 +13695,20 @@
       <c r="O116" s="17"/>
     </row>
     <row r="117" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
-      <c r="A117" s="14"/>
-      <c r="B117" s="15" t="s">
-        <v>963</v>
-      </c>
-      <c r="C117" s="21" t="s">
+      <c r="A117" s="74" t="s">
+        <v>980</v>
+      </c>
+      <c r="B117" s="79" t="s">
+        <v>974</v>
+      </c>
+      <c r="C117" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D117" s="22" t="s">
+      <c r="D117" s="66" t="s">
         <v>253</v>
       </c>
-      <c r="E117" s="22" t="s">
-        <v>969</v>
+      <c r="E117" s="66" t="s">
+        <v>981</v>
       </c>
       <c r="F117" s="22"/>
       <c r="G117" s="22"/>
@@ -13627,7 +13724,7 @@
     <row r="118" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A118" s="14"/>
       <c r="B118" s="15" t="s">
-        <v>970</v>
+        <v>982</v>
       </c>
       <c r="C118" s="21" t="s">
         <v>30</v>
@@ -13636,10 +13733,10 @@
         <v>711</v>
       </c>
       <c r="E118" s="22" t="s">
-        <v>971</v>
+        <v>983</v>
       </c>
       <c r="F118" s="22" t="s">
-        <v>972</v>
+        <v>984</v>
       </c>
       <c r="G118" s="22"/>
       <c r="H118" s="22"/>
@@ -13654,7 +13751,7 @@
     <row r="119" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A119" s="14"/>
       <c r="B119" s="15" t="s">
-        <v>973</v>
+        <v>985</v>
       </c>
       <c r="C119" s="21" t="s">
         <v>30</v>
@@ -13663,10 +13760,10 @@
         <v>576</v>
       </c>
       <c r="E119" s="22" t="s">
-        <v>974</v>
+        <v>986</v>
       </c>
       <c r="F119" s="22" t="s">
-        <v>916</v>
+        <v>926</v>
       </c>
       <c r="G119" s="22"/>
       <c r="H119" s="22"/>
@@ -13681,7 +13778,7 @@
     <row r="120" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A120" s="14"/>
       <c r="B120" s="15" t="s">
-        <v>975</v>
+        <v>987</v>
       </c>
       <c r="C120" s="21" t="s">
         <v>30</v>
@@ -13690,10 +13787,10 @@
         <v>493</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>976</v>
+        <v>988</v>
       </c>
       <c r="F120" s="22" t="s">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="G120" s="22"/>
       <c r="H120" s="22"/>
@@ -13708,7 +13805,7 @@
     <row r="121" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A121" s="14"/>
       <c r="B121" s="15" t="s">
-        <v>977</v>
+        <v>989</v>
       </c>
       <c r="C121" s="21" t="s">
         <v>5</v>
@@ -13717,10 +13814,10 @@
         <v>49</v>
       </c>
       <c r="E121" s="22" t="s">
-        <v>978</v>
+        <v>990</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>979</v>
+        <v>991</v>
       </c>
       <c r="G121" s="22"/>
       <c r="H121" s="22"/>
@@ -13759,7 +13856,7 @@
     <row r="123" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A123" s="14"/>
       <c r="B123" s="15" t="s">
-        <v>980</v>
+        <v>992</v>
       </c>
       <c r="C123" s="21" t="s">
         <v>30</v>
@@ -13768,10 +13865,10 @@
         <v>711</v>
       </c>
       <c r="E123" s="22" t="s">
-        <v>971</v>
+        <v>983</v>
       </c>
       <c r="F123" s="22" t="s">
-        <v>981</v>
+        <v>993</v>
       </c>
       <c r="G123" s="22"/>
       <c r="H123" s="22"/>
@@ -13786,7 +13883,7 @@
     <row r="124" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A124" s="14"/>
       <c r="B124" s="15" t="s">
-        <v>973</v>
+        <v>985</v>
       </c>
       <c r="C124" s="21" t="s">
         <v>30</v>
@@ -13795,10 +13892,10 @@
         <v>576</v>
       </c>
       <c r="E124" s="22" t="s">
-        <v>974</v>
+        <v>986</v>
       </c>
       <c r="F124" s="22" t="s">
-        <v>916</v>
+        <v>926</v>
       </c>
       <c r="G124" s="22"/>
       <c r="H124" s="22"/>
@@ -13813,7 +13910,7 @@
     <row r="125" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A125" s="14"/>
       <c r="B125" s="15" t="s">
-        <v>975</v>
+        <v>987</v>
       </c>
       <c r="C125" s="21" t="s">
         <v>30</v>
@@ -13822,10 +13919,10 @@
         <v>493</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>982</v>
+        <v>994</v>
       </c>
       <c r="F125" s="22" t="s">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="G125" s="22"/>
       <c r="H125" s="22"/>
@@ -13840,7 +13937,7 @@
     <row r="126" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A126" s="14"/>
       <c r="B126" s="15" t="s">
-        <v>977</v>
+        <v>989</v>
       </c>
       <c r="C126" s="21" t="s">
         <v>5</v>
@@ -13849,10 +13946,10 @@
         <v>49</v>
       </c>
       <c r="E126" s="22" t="s">
-        <v>978</v>
+        <v>990</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>983</v>
+        <v>995</v>
       </c>
       <c r="G126" s="22"/>
       <c r="H126" s="22"/>
@@ -13866,10 +13963,10 @@
     </row>
     <row r="127" customFormat="1" ht="15.5" spans="1:6">
       <c r="A127" s="27" t="s">
-        <v>984</v>
+        <v>996</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>985</v>
+        <v>997</v>
       </c>
       <c r="C127" s="21" t="s">
         <v>12</v>
@@ -13878,7 +13975,7 @@
         <v>297</v>
       </c>
       <c r="E127" t="s">
-        <v>930</v>
+        <v>940</v>
       </c>
       <c r="F127" t="b">
         <v>0</v>
@@ -16499,7 +16596,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.0833333333333" defaultRowHeight="15.5"/>
@@ -16621,7 +16718,7 @@
     </row>
     <row r="5" s="6" customFormat="1" ht="42" spans="1:15">
       <c r="A5" s="27" t="s">
-        <v>986</v>
+        <v>998</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>761</v>
@@ -16650,7 +16747,7 @@
     </row>
     <row r="6" s="5" customFormat="1" spans="2:15">
       <c r="B6" s="20" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>30</v>
@@ -16659,7 +16756,7 @@
         <v>576</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="F6" s="23">
         <v>2000</v>
@@ -16677,7 +16774,7 @@
     <row r="7" s="5" customFormat="1" spans="1:15">
       <c r="A7" s="27"/>
       <c r="B7" s="20" t="s">
-        <v>942</v>
+        <v>953</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>30</v>
@@ -16686,10 +16783,10 @@
         <v>363</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>987</v>
+        <v>999</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>916</v>
+        <v>926</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -16713,7 +16810,7 @@
         <v>714</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>883</v>
+        <v>889</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
@@ -16728,7 +16825,7 @@
     <row r="9" s="5" customFormat="1" spans="1:15">
       <c r="A9" s="27"/>
       <c r="B9" s="20" t="s">
-        <v>942</v>
+        <v>953</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>30</v>
@@ -16737,10 +16834,10 @@
         <v>706</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>987</v>
+        <v>999</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>988</v>
+        <v>1000</v>
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
@@ -16764,7 +16861,7 @@
         <v>714</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>883</v>
+        <v>889</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
@@ -16779,7 +16876,7 @@
     <row r="11" s="5" customFormat="1" spans="1:15">
       <c r="A11" s="27"/>
       <c r="B11" s="20" t="s">
-        <v>989</v>
+        <v>1001</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>8</v>
@@ -16788,10 +16885,10 @@
         <v>656</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>923</v>
+        <v>933</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>990</v>
+        <v>1002</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
@@ -16806,7 +16903,7 @@
     <row r="12" s="5" customFormat="1" spans="1:15">
       <c r="A12" s="27"/>
       <c r="B12" s="20" t="s">
-        <v>890</v>
+        <v>898</v>
       </c>
       <c r="C12" s="43" t="s">
         <v>30</v>
@@ -16815,7 +16912,7 @@
         <v>576</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>891</v>
+        <v>899</v>
       </c>
       <c r="F12" s="45">
         <v>1000</v>
@@ -17614,7 +17711,7 @@
     </row>
     <row r="5" s="4" customFormat="1" ht="14.5" spans="1:15">
       <c r="A5" s="14" t="s">
-        <v>991</v>
+        <v>1003</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>750</v>
@@ -17632,7 +17729,7 @@
         <v>752</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>944</v>
+        <v>955</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>754</v>
@@ -17701,7 +17798,7 @@
     <row r="8" s="6" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A8" s="14"/>
       <c r="B8" s="15" t="s">
-        <v>955</v>
+        <v>966</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>30</v>
@@ -17778,7 +17875,7 @@
     <row r="11" s="5" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A11" s="14"/>
       <c r="B11" s="15" t="s">
-        <v>956</v>
+        <v>967</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>30</v>
@@ -17787,7 +17884,7 @@
         <v>576</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>957</v>
+        <v>968</v>
       </c>
       <c r="F11" s="23">
         <v>3000</v>
@@ -17805,7 +17902,7 @@
     <row r="12" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
-        <v>973</v>
+        <v>985</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>30</v>
@@ -17814,10 +17911,10 @@
         <v>576</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>974</v>
+        <v>986</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>916</v>
+        <v>926</v>
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
@@ -17832,7 +17929,7 @@
     <row r="13" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
-        <v>975</v>
+        <v>987</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>30</v>
@@ -17841,10 +17938,10 @@
         <v>493</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>976</v>
+        <v>988</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
@@ -17859,7 +17956,7 @@
     <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
-        <v>977</v>
+        <v>989</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>5</v>
@@ -17868,10 +17965,10 @@
         <v>49</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>978</v>
+        <v>990</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>979</v>
+        <v>991</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
@@ -17910,7 +18007,7 @@
     <row r="16" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>980</v>
+        <v>992</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>30</v>
@@ -17919,10 +18016,10 @@
         <v>711</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>971</v>
+        <v>983</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>981</v>
+        <v>993</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
@@ -17937,7 +18034,7 @@
     <row r="17" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>973</v>
+        <v>985</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>30</v>
@@ -17946,10 +18043,10 @@
         <v>576</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>974</v>
+        <v>986</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>916</v>
+        <v>926</v>
       </c>
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
@@ -17964,7 +18061,7 @@
     <row r="18" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>975</v>
+        <v>987</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>30</v>
@@ -17973,10 +18070,10 @@
         <v>493</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>982</v>
+        <v>994</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
@@ -17991,7 +18088,7 @@
     <row r="19" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>977</v>
+        <v>989</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>5</v>
@@ -18000,10 +18097,10 @@
         <v>49</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>978</v>
+        <v>990</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>983</v>
+        <v>995</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>

</xml_diff>

<commit_message>
Mobile purchase and sale order
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-Settings.xlsx
+++ b/tests/artifact/script/UI-Settings.xlsx
@@ -10673,9 +10673,9 @@
   <dimension ref="A1:O290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
+      <selection pane="bottomLeft" activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>

</xml_diff>